<commit_message>
new cameras added to the list of possibilities
</commit_message>
<xml_diff>
--- a/docs/Gimbal_Camera_Possibilities.xlsx
+++ b/docs/Gimbal_Camera_Possibilities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferra\OneDrive\Desktop\thws\Robotics Project - Hawkeye System\Hawkeye_System\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5F838C-BA1E-40CF-8697-185CE5967332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3FC319-BDD5-4846-BB3D-6B661FD437E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8E4CF4B1-C19C-4AE2-898C-70AF66287E7B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="99">
   <si>
     <t>Camera</t>
   </si>
@@ -246,6 +246,96 @@
   </si>
   <si>
     <t>USB 2 / 3</t>
+  </si>
+  <si>
+    <t>Camera Model</t>
+  </si>
+  <si>
+    <t>FPS</t>
+  </si>
+  <si>
+    <t>Size (mm)</t>
+  </si>
+  <si>
+    <t>E-Con AR0234</t>
+  </si>
+  <si>
+    <t>1920×1200 (2.3 MP)</t>
+  </si>
+  <si>
+    <t>~30 x 30</t>
+  </si>
+  <si>
+    <t>E-Con OV2312</t>
+  </si>
+  <si>
+    <t>1600×1300 (2 MP)</t>
+  </si>
+  <si>
+    <t>Arducam B0385 (OV9281)</t>
+  </si>
+  <si>
+    <t>1280×800 (1 MP)</t>
+  </si>
+  <si>
+    <t>24 x 24</t>
+  </si>
+  <si>
+    <t>E-Con IMX900</t>
+  </si>
+  <si>
+    <t>Newer, solid choice, mid-range FPS</t>
+  </si>
+  <si>
+    <t>E-Con IMX264</t>
+  </si>
+  <si>
+    <t>2448×2048 (5 MP)</t>
+  </si>
+  <si>
+    <t>Large, premium image quality, overkill for Pi</t>
+  </si>
+  <si>
+    <t>Price (USD)</t>
+  </si>
+  <si>
+    <t>USB 3.1 Gen 1 device</t>
+  </si>
+  <si>
+    <t>~30 x 30 x 26</t>
+  </si>
+  <si>
+    <t>Best performance/resolution tradeoff, great Pi support</t>
+  </si>
+  <si>
+    <t>Dual RGB+IR, smaller, good fusion with thermal cam</t>
+  </si>
+  <si>
+    <t>Tiny, best for size-constrained gimbals, Pi-friendly</t>
+  </si>
+  <si>
+    <t>USB 3.2 Gen 1 device</t>
+  </si>
+  <si>
+    <t>1920×1200 (3.2 MP)</t>
+  </si>
+  <si>
+    <t>72 (€)</t>
+  </si>
+  <si>
+    <t>40 x 40</t>
+  </si>
+  <si>
+    <t>145 fps</t>
+  </si>
+  <si>
+    <t>117 fps</t>
+  </si>
+  <si>
+    <t>Launching soon</t>
+  </si>
+  <si>
+    <t>Pick</t>
   </si>
 </sst>
 </file>
@@ -319,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -333,11 +423,29 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -674,15 +782,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A4194D-159D-4E87-8F87-5CC789B37907}">
-  <dimension ref="B2:I15"/>
+  <dimension ref="A2:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="I23" sqref="A18:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -1031,26 +1140,200 @@
       <c r="B15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="4">
         <v>175</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="4" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>1</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="13">
+        <v>26</v>
+      </c>
+      <c r="H19" s="13">
+        <v>184</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>2</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="13">
+        <v>20</v>
+      </c>
+      <c r="H20" s="13">
+        <v>229</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>3</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>4</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>5</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="13">
+        <v>699</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1069,6 +1352,11 @@
     <hyperlink ref="B13" r:id="rId11" xr:uid="{A72BAFDB-0B0C-4064-93F3-8A1AD838363C}"/>
     <hyperlink ref="B14" r:id="rId12" xr:uid="{569A44BE-4B3F-4A32-B855-2FA7CBD46CA1}"/>
     <hyperlink ref="B15" r:id="rId13" xr:uid="{D0887847-C9BD-4B0B-AFD9-ACD9266FA706}"/>
+    <hyperlink ref="B19" r:id="rId14" display="https://www.e-consystems.com/industrial-cameras/ar0234-usb3-global-shutter-camera.asp" xr:uid="{3FC5564A-4A8A-4792-B8A1-A001F9C0EEEA}"/>
+    <hyperlink ref="B20" r:id="rId15" display="https://www.e-consystems.com/usb-cameras/2mp-ov2312-global-shutter-rgb-ir-camera.asp" xr:uid="{EED2E95B-0A0B-4727-A75B-642F6FC309EC}"/>
+    <hyperlink ref="B21" r:id="rId16" display="https://www.welectron.com/Arducam-B0385-120fps-Global-Shutter-Color-USB-Camera-Board?utm_source=chatgpt.com" xr:uid="{9DB4DF35-089D-4F99-A459-211FA7BFD837}"/>
+    <hyperlink ref="B22" r:id="rId17" display="https://www.e-consystems.com/usb-cameras/sony-imx900-global-shutter-camera.asp" xr:uid="{84231794-CE2D-47C6-A7C2-7BA76FE164A7}"/>
+    <hyperlink ref="B23" r:id="rId18" display="https://www.e-consystems.com/sony-imx264-camera.asp" xr:uid="{6754D5C6-2CA5-442F-AA35-71BEA1D917CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>